<commit_message>
added lat long to picks
</commit_message>
<xml_diff>
--- a/TCCZ_krig/picks_nearF.xlsx
+++ b/TCCZ_krig/picks_nearF.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7740"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="point_nearF" sheetId="1" r:id="rId1"/>
+    <sheet name="point_nearF (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="137">
   <si>
     <t>UWI</t>
   </si>
@@ -756,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5000,4 +5001,4888 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L128"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>437287.87</v>
+      </c>
+      <c r="C2">
+        <v>3682412.68</v>
+      </c>
+      <c r="D2">
+        <v>-81.673275052500003</v>
+      </c>
+      <c r="E2">
+        <v>33.280813896200002</v>
+      </c>
+      <c r="F2">
+        <v>278.25</v>
+      </c>
+      <c r="G2">
+        <v>254</v>
+      </c>
+      <c r="H2">
+        <v>200</v>
+      </c>
+      <c r="I2">
+        <v>191.25</v>
+      </c>
+      <c r="J2">
+        <v>8.75</v>
+      </c>
+      <c r="K2">
+        <v>149.25</v>
+      </c>
+      <c r="L2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>436497.6</v>
+      </c>
+      <c r="C3">
+        <v>3682296.07</v>
+      </c>
+      <c r="D3">
+        <v>-81.681752942800003</v>
+      </c>
+      <c r="E3">
+        <v>33.2797158411</v>
+      </c>
+      <c r="F3">
+        <v>293.89999999999998</v>
+      </c>
+      <c r="G3">
+        <v>270</v>
+      </c>
+      <c r="H3">
+        <v>178.9</v>
+      </c>
+      <c r="I3">
+        <v>165.9</v>
+      </c>
+      <c r="J3">
+        <v>13</v>
+      </c>
+      <c r="K3">
+        <v>140</v>
+      </c>
+      <c r="L3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>436307.51</v>
+      </c>
+      <c r="C4">
+        <v>3682353.98</v>
+      </c>
+      <c r="D4">
+        <v>-81.683798202399998</v>
+      </c>
+      <c r="E4">
+        <v>33.280226927699999</v>
+      </c>
+      <c r="F4">
+        <v>289.60000000000002</v>
+      </c>
+      <c r="G4">
+        <v>273</v>
+      </c>
+      <c r="H4">
+        <v>202</v>
+      </c>
+      <c r="I4">
+        <v>189.6</v>
+      </c>
+      <c r="J4">
+        <v>12.4</v>
+      </c>
+      <c r="K4">
+        <v>158</v>
+      </c>
+      <c r="L4">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>436158.97</v>
+      </c>
+      <c r="C5">
+        <v>3682265.41</v>
+      </c>
+      <c r="D5">
+        <v>-81.685387002499994</v>
+      </c>
+      <c r="E5">
+        <v>33.279419289000003</v>
+      </c>
+      <c r="F5">
+        <v>277.39999999999998</v>
+      </c>
+      <c r="G5">
+        <v>272</v>
+      </c>
+      <c r="H5">
+        <v>205</v>
+      </c>
+      <c r="I5">
+        <v>200.4</v>
+      </c>
+      <c r="J5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="K5">
+        <v>159</v>
+      </c>
+      <c r="L5">
+        <v>127.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>436669.33600000001</v>
+      </c>
+      <c r="C6">
+        <v>3681492.08</v>
+      </c>
+      <c r="D6">
+        <v>-81.679852695999998</v>
+      </c>
+      <c r="E6">
+        <v>33.272474465800002</v>
+      </c>
+      <c r="F6">
+        <v>254.10000600000001</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>168</v>
+      </c>
+      <c r="I6">
+        <v>151</v>
+      </c>
+      <c r="J6">
+        <v>17</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>436642</v>
+      </c>
+      <c r="C7">
+        <v>3682574</v>
+      </c>
+      <c r="D7">
+        <v>-81.680221790299996</v>
+      </c>
+      <c r="E7">
+        <v>33.282231097699999</v>
+      </c>
+      <c r="F7">
+        <v>298</v>
+      </c>
+      <c r="G7">
+        <v>264</v>
+      </c>
+      <c r="H7">
+        <v>197</v>
+      </c>
+      <c r="I7">
+        <v>187</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>153</v>
+      </c>
+      <c r="L7">
+        <v>123.036</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>436648.6</v>
+      </c>
+      <c r="C8">
+        <v>3682382</v>
+      </c>
+      <c r="D8">
+        <v>-81.680137502799994</v>
+      </c>
+      <c r="E8">
+        <v>33.2804997677</v>
+      </c>
+      <c r="F8">
+        <v>284</v>
+      </c>
+      <c r="G8">
+        <v>250</v>
+      </c>
+      <c r="H8">
+        <v>196</v>
+      </c>
+      <c r="I8">
+        <v>191</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>163</v>
+      </c>
+      <c r="L8">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>436651.94400000002</v>
+      </c>
+      <c r="C9">
+        <v>3682161.7110000001</v>
+      </c>
+      <c r="D9">
+        <v>-81.680086205699993</v>
+      </c>
+      <c r="E9">
+        <v>33.278513096600001</v>
+      </c>
+      <c r="F9">
+        <v>292</v>
+      </c>
+      <c r="G9">
+        <v>244</v>
+      </c>
+      <c r="H9">
+        <v>189</v>
+      </c>
+      <c r="I9">
+        <v>182</v>
+      </c>
+      <c r="J9">
+        <v>7</v>
+      </c>
+      <c r="K9">
+        <v>155</v>
+      </c>
+      <c r="L9">
+        <v>122.741</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>436564.87300000002</v>
+      </c>
+      <c r="C10">
+        <v>3681240.0789999999</v>
+      </c>
+      <c r="D10">
+        <v>-81.680956709900002</v>
+      </c>
+      <c r="E10">
+        <v>33.270195428400001</v>
+      </c>
+      <c r="F10">
+        <v>224.17</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>181.75</v>
+      </c>
+      <c r="I10">
+        <v>163</v>
+      </c>
+      <c r="J10">
+        <v>18.75</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>436638.21</v>
+      </c>
+      <c r="C11">
+        <v>3681157.14</v>
+      </c>
+      <c r="D11">
+        <v>-81.680163507499998</v>
+      </c>
+      <c r="E11">
+        <v>33.269451684300002</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>179</v>
+      </c>
+      <c r="I11">
+        <v>162</v>
+      </c>
+      <c r="J11">
+        <v>17</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>436579.96</v>
+      </c>
+      <c r="C12">
+        <v>3681181.59</v>
+      </c>
+      <c r="D12">
+        <v>-81.680790634100006</v>
+      </c>
+      <c r="E12">
+        <v>33.2696687818</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>188</v>
+      </c>
+      <c r="I12">
+        <v>168</v>
+      </c>
+      <c r="J12">
+        <v>20</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>436556.04</v>
+      </c>
+      <c r="C13">
+        <v>3681106.64</v>
+      </c>
+      <c r="D13">
+        <v>-81.681042217500007</v>
+      </c>
+      <c r="E13">
+        <v>33.268991371200002</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>187</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>436489.38</v>
+      </c>
+      <c r="C14">
+        <v>3681213.49</v>
+      </c>
+      <c r="D14">
+        <v>-81.681765407100002</v>
+      </c>
+      <c r="E14">
+        <v>33.269951165599998</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>178</v>
+      </c>
+      <c r="I14">
+        <v>159</v>
+      </c>
+      <c r="J14">
+        <v>19</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>436481.41</v>
+      </c>
+      <c r="C15">
+        <v>3681098.67</v>
+      </c>
+      <c r="D15">
+        <v>-81.681842941200003</v>
+      </c>
+      <c r="E15">
+        <v>33.2689150908</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>189</v>
+      </c>
+      <c r="I15">
+        <v>161</v>
+      </c>
+      <c r="J15">
+        <v>28</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>436452.06</v>
+      </c>
+      <c r="C16">
+        <v>3681102.82</v>
+      </c>
+      <c r="D16">
+        <v>-81.682158354400002</v>
+      </c>
+      <c r="E16">
+        <v>33.268950791000002</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>185</v>
+      </c>
+      <c r="I16">
+        <v>160</v>
+      </c>
+      <c r="J16">
+        <v>25</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>436449.51</v>
+      </c>
+      <c r="C17">
+        <v>3681067.41</v>
+      </c>
+      <c r="D17">
+        <v>-81.682183252800002</v>
+      </c>
+      <c r="E17">
+        <v>33.2686312644</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>184</v>
+      </c>
+      <c r="I17">
+        <v>158</v>
+      </c>
+      <c r="J17">
+        <v>26</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>436476.3</v>
+      </c>
+      <c r="C18">
+        <v>3681049.87</v>
+      </c>
+      <c r="D18">
+        <v>-81.681894389099995</v>
+      </c>
+      <c r="E18">
+        <v>33.268474643899999</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>167</v>
+      </c>
+      <c r="I18">
+        <v>150</v>
+      </c>
+      <c r="J18">
+        <v>17</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>436505.01</v>
+      </c>
+      <c r="C19">
+        <v>3681009.69</v>
+      </c>
+      <c r="D19">
+        <v>-81.681583327799999</v>
+      </c>
+      <c r="E19">
+        <v>33.268113937000003</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>168</v>
+      </c>
+      <c r="I19">
+        <v>145</v>
+      </c>
+      <c r="J19">
+        <v>23</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>436470.88</v>
+      </c>
+      <c r="C20">
+        <v>3680983.21</v>
+      </c>
+      <c r="D20">
+        <v>-81.6819479145</v>
+      </c>
+      <c r="E20">
+        <v>33.267873092499997</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>436675.15</v>
+      </c>
+      <c r="C21">
+        <v>3681322.82</v>
+      </c>
+      <c r="D21">
+        <v>-81.679778455100006</v>
+      </c>
+      <c r="E21">
+        <v>33.270948187000002</v>
+      </c>
+      <c r="F21">
+        <v>237.47</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>179</v>
+      </c>
+      <c r="I21">
+        <v>160.5</v>
+      </c>
+      <c r="J21">
+        <v>18.5</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <v>436429.74</v>
+      </c>
+      <c r="C22">
+        <v>3680950.36</v>
+      </c>
+      <c r="D22">
+        <v>-81.682387316100005</v>
+      </c>
+      <c r="E22">
+        <v>33.267574380100001</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>160</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23">
+        <v>436430.2</v>
+      </c>
+      <c r="C23">
+        <v>3681022.17</v>
+      </c>
+      <c r="D23">
+        <v>-81.682387408400004</v>
+      </c>
+      <c r="E23">
+        <v>33.268222088900004</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24">
+        <v>436394.02</v>
+      </c>
+      <c r="C24">
+        <v>3681037.75</v>
+      </c>
+      <c r="D24">
+        <v>-81.682776951700006</v>
+      </c>
+      <c r="E24">
+        <v>33.268360476200002</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>179</v>
+      </c>
+      <c r="I24">
+        <v>156</v>
+      </c>
+      <c r="J24">
+        <v>23</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <v>436374.24</v>
+      </c>
+      <c r="C25">
+        <v>3681013.83</v>
+      </c>
+      <c r="D25">
+        <v>-81.682987645200001</v>
+      </c>
+      <c r="E25">
+        <v>33.268143565099997</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26">
+        <v>436741.35100000002</v>
+      </c>
+      <c r="C26">
+        <v>3681344.4160000002</v>
+      </c>
+      <c r="D26">
+        <v>-81.679069162999994</v>
+      </c>
+      <c r="E26">
+        <v>33.2711468579</v>
+      </c>
+      <c r="F26">
+        <v>235.65</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>168</v>
+      </c>
+      <c r="I26">
+        <v>150</v>
+      </c>
+      <c r="J26">
+        <v>18</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27">
+        <v>436816.54700000002</v>
+      </c>
+      <c r="C27">
+        <v>3681309.2740000002</v>
+      </c>
+      <c r="D27">
+        <v>-81.678259336500005</v>
+      </c>
+      <c r="E27">
+        <v>33.270834310399998</v>
+      </c>
+      <c r="F27">
+        <v>223.07</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>172</v>
+      </c>
+      <c r="I27">
+        <v>156.5</v>
+      </c>
+      <c r="J27">
+        <v>15.5</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28">
+        <v>436873.245</v>
+      </c>
+      <c r="C28">
+        <v>3681299.5529999998</v>
+      </c>
+      <c r="D28">
+        <v>-81.677649896099993</v>
+      </c>
+      <c r="E28">
+        <v>33.270749955799999</v>
+      </c>
+      <c r="F28">
+        <v>216.4</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>169.5</v>
+      </c>
+      <c r="I28">
+        <v>157</v>
+      </c>
+      <c r="J28">
+        <v>12.5</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29">
+        <v>436836.071</v>
+      </c>
+      <c r="C29">
+        <v>3681382.142</v>
+      </c>
+      <c r="D29">
+        <v>-81.678054781699998</v>
+      </c>
+      <c r="E29">
+        <v>33.271492679700003</v>
+      </c>
+      <c r="F29">
+        <v>224.7</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>168</v>
+      </c>
+      <c r="I29">
+        <v>156</v>
+      </c>
+      <c r="J29">
+        <v>12</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30">
+        <v>436736</v>
+      </c>
+      <c r="C30">
+        <v>3681651</v>
+      </c>
+      <c r="D30">
+        <v>-81.679147997900003</v>
+      </c>
+      <c r="E30">
+        <v>33.273911742000003</v>
+      </c>
+      <c r="F30">
+        <v>239</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>170</v>
+      </c>
+      <c r="I30">
+        <v>158</v>
+      </c>
+      <c r="J30">
+        <v>12</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31">
+        <v>437038.98</v>
+      </c>
+      <c r="C31">
+        <v>3681393.07</v>
+      </c>
+      <c r="D31">
+        <v>-81.6758768981</v>
+      </c>
+      <c r="E31">
+        <v>33.271603118599998</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>179</v>
+      </c>
+      <c r="I31">
+        <v>164</v>
+      </c>
+      <c r="J31">
+        <v>15</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32">
+        <v>436917.13</v>
+      </c>
+      <c r="C32">
+        <v>3681415.9</v>
+      </c>
+      <c r="D32">
+        <v>-81.677186795599994</v>
+      </c>
+      <c r="E32">
+        <v>33.271801904699998</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>171</v>
+      </c>
+      <c r="I32">
+        <v>159</v>
+      </c>
+      <c r="J32">
+        <v>12</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33">
+        <v>436781.02</v>
+      </c>
+      <c r="C33">
+        <v>3681421.4</v>
+      </c>
+      <c r="D33">
+        <v>-81.678648601999996</v>
+      </c>
+      <c r="E33">
+        <v>33.271843534299997</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>177</v>
+      </c>
+      <c r="I33">
+        <v>165</v>
+      </c>
+      <c r="J33">
+        <v>12</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34">
+        <v>437006.25</v>
+      </c>
+      <c r="C34">
+        <v>3681589.13</v>
+      </c>
+      <c r="D34">
+        <v>-81.676241936799997</v>
+      </c>
+      <c r="E34">
+        <v>33.273369547400002</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>178</v>
+      </c>
+      <c r="I34">
+        <v>161</v>
+      </c>
+      <c r="J34">
+        <v>17</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35">
+        <v>437034.83</v>
+      </c>
+      <c r="C35">
+        <v>3681653.04</v>
+      </c>
+      <c r="D35">
+        <v>-81.675939501900004</v>
+      </c>
+      <c r="E35">
+        <v>33.273947647100002</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>179</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36">
+        <v>436789.41</v>
+      </c>
+      <c r="C36">
+        <v>3681804.82</v>
+      </c>
+      <c r="D36">
+        <v>-81.6785852366</v>
+      </c>
+      <c r="E36">
+        <v>33.275302238000002</v>
+      </c>
+      <c r="F36">
+        <v>275.79998799999998</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>165.5</v>
+      </c>
+      <c r="I36">
+        <v>150.5</v>
+      </c>
+      <c r="J36">
+        <v>15</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37">
+        <v>436898.02</v>
+      </c>
+      <c r="C37">
+        <v>3681966.45</v>
+      </c>
+      <c r="D37">
+        <v>-81.677430281699998</v>
+      </c>
+      <c r="E37">
+        <v>33.276766407799997</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>186</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38">
+        <v>436855.77</v>
+      </c>
+      <c r="C38">
+        <v>3682006.23</v>
+      </c>
+      <c r="D38">
+        <v>-81.677886718400003</v>
+      </c>
+      <c r="E38">
+        <v>33.277122722900003</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39">
+        <v>436741.14</v>
+      </c>
+      <c r="C39">
+        <v>3681167.18</v>
+      </c>
+      <c r="D39">
+        <v>-81.679059070299999</v>
+      </c>
+      <c r="E39">
+        <v>33.269548285699997</v>
+      </c>
+      <c r="F39">
+        <v>205</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>182</v>
+      </c>
+      <c r="I39">
+        <v>164</v>
+      </c>
+      <c r="J39">
+        <v>18</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40">
+        <v>436743.77</v>
+      </c>
+      <c r="C40">
+        <v>3681058.99</v>
+      </c>
+      <c r="D40">
+        <v>-81.679023289499995</v>
+      </c>
+      <c r="E40">
+        <v>33.268572632599998</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41">
+        <v>436747.97</v>
+      </c>
+      <c r="C41">
+        <v>3680950.52</v>
+      </c>
+      <c r="D41">
+        <v>-81.678970633800006</v>
+      </c>
+      <c r="E41">
+        <v>33.267594545900003</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42">
+        <v>436673.9</v>
+      </c>
+      <c r="C42">
+        <v>3681588.23</v>
+      </c>
+      <c r="D42">
+        <v>-81.679810403900007</v>
+      </c>
+      <c r="E42">
+        <v>33.273341947399999</v>
+      </c>
+      <c r="F42">
+        <v>276.05999800000001</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>161</v>
+      </c>
+      <c r="I42">
+        <v>151</v>
+      </c>
+      <c r="J42">
+        <v>10</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43">
+        <v>436595.07</v>
+      </c>
+      <c r="C43">
+        <v>3681595.68</v>
+      </c>
+      <c r="D43">
+        <v>-81.6806573426</v>
+      </c>
+      <c r="E43">
+        <v>33.2734045057</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>174</v>
+      </c>
+      <c r="I43">
+        <v>156</v>
+      </c>
+      <c r="J43">
+        <v>18</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44">
+        <v>436548.86</v>
+      </c>
+      <c r="C44">
+        <v>3681520.58</v>
+      </c>
+      <c r="D44">
+        <v>-81.6811482584</v>
+      </c>
+      <c r="E44">
+        <v>33.2727244302</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>165</v>
+      </c>
+      <c r="I44">
+        <v>147</v>
+      </c>
+      <c r="J44">
+        <v>18</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45">
+        <v>436530.73</v>
+      </c>
+      <c r="C45">
+        <v>3681334.99</v>
+      </c>
+      <c r="D45">
+        <v>-81.681329938800005</v>
+      </c>
+      <c r="E45">
+        <v>33.271049456299998</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>171</v>
+      </c>
+      <c r="I45">
+        <v>154</v>
+      </c>
+      <c r="J45">
+        <v>17</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46">
+        <v>436617.6</v>
+      </c>
+      <c r="C46">
+        <v>3681185.24</v>
+      </c>
+      <c r="D46">
+        <v>-81.680386755599997</v>
+      </c>
+      <c r="E46">
+        <v>33.269703917000001</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>186</v>
+      </c>
+      <c r="I46">
+        <v>168</v>
+      </c>
+      <c r="J46">
+        <v>18</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47">
+        <v>436350.5</v>
+      </c>
+      <c r="C47">
+        <v>3680998.7</v>
+      </c>
+      <c r="D47">
+        <v>-81.683241471100004</v>
+      </c>
+      <c r="E47">
+        <v>33.2680057002</v>
+      </c>
+      <c r="F47">
+        <v>215.89999399999999</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>182</v>
+      </c>
+      <c r="I47">
+        <v>172</v>
+      </c>
+      <c r="J47">
+        <v>10</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48">
+        <v>436355.27</v>
+      </c>
+      <c r="C48">
+        <v>3681230.56</v>
+      </c>
+      <c r="D48">
+        <v>-81.683206521900004</v>
+      </c>
+      <c r="E48">
+        <v>33.270097214300002</v>
+      </c>
+      <c r="F48">
+        <v>234.39999399999999</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>166</v>
+      </c>
+      <c r="I48">
+        <v>153</v>
+      </c>
+      <c r="J48">
+        <v>13</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49">
+        <v>436388.96</v>
+      </c>
+      <c r="C49">
+        <v>3681491.67</v>
+      </c>
+      <c r="D49">
+        <v>-81.682863105899997</v>
+      </c>
+      <c r="E49">
+        <v>33.272454252099998</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>167</v>
+      </c>
+      <c r="I49">
+        <v>148</v>
+      </c>
+      <c r="J49">
+        <v>19</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50">
+        <v>436265.07</v>
+      </c>
+      <c r="C50">
+        <v>3681173.02</v>
+      </c>
+      <c r="D50">
+        <v>-81.6841709439</v>
+      </c>
+      <c r="E50">
+        <v>33.269572908800001</v>
+      </c>
+      <c r="F50">
+        <v>240.10000600000001</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>177</v>
+      </c>
+      <c r="I50">
+        <v>164</v>
+      </c>
+      <c r="J50">
+        <v>13</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51">
+        <v>436187.41</v>
+      </c>
+      <c r="C51">
+        <v>3681356.59</v>
+      </c>
+      <c r="D51">
+        <v>-81.685017674600005</v>
+      </c>
+      <c r="E51">
+        <v>33.2712239986</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>171</v>
+      </c>
+      <c r="I51">
+        <v>154</v>
+      </c>
+      <c r="J51">
+        <v>17</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52">
+        <v>436140.72</v>
+      </c>
+      <c r="C52">
+        <v>3681096.66</v>
+      </c>
+      <c r="D52">
+        <v>-81.685500688800005</v>
+      </c>
+      <c r="E52">
+        <v>33.268876828499998</v>
+      </c>
+      <c r="F52">
+        <v>256.459991</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>189</v>
+      </c>
+      <c r="I52">
+        <v>174</v>
+      </c>
+      <c r="J52">
+        <v>15</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53">
+        <v>436493.34</v>
+      </c>
+      <c r="C53">
+        <v>3681110.73</v>
+      </c>
+      <c r="D53">
+        <v>-81.681715696300003</v>
+      </c>
+      <c r="E53">
+        <v>33.269024567599999</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>187</v>
+      </c>
+      <c r="I53">
+        <v>160</v>
+      </c>
+      <c r="J53">
+        <v>27</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54">
+        <v>436961.62</v>
+      </c>
+      <c r="C54">
+        <v>3681735.18</v>
+      </c>
+      <c r="D54">
+        <v>-81.676731291199999</v>
+      </c>
+      <c r="E54">
+        <v>33.274684218499999</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>178</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55">
+        <v>436143.41</v>
+      </c>
+      <c r="C55">
+        <v>3680736.15</v>
+      </c>
+      <c r="D55">
+        <v>-81.685446436199996</v>
+      </c>
+      <c r="E55">
+        <v>33.265625414100001</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>172</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56">
+        <v>436018.32</v>
+      </c>
+      <c r="C56">
+        <v>3681471.32</v>
+      </c>
+      <c r="D56">
+        <v>-81.686841283199996</v>
+      </c>
+      <c r="E56">
+        <v>33.2722487634</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>183</v>
+      </c>
+      <c r="I56">
+        <v>172</v>
+      </c>
+      <c r="J56">
+        <v>11</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57">
+        <v>436296.19</v>
+      </c>
+      <c r="C57">
+        <v>3681583.07</v>
+      </c>
+      <c r="D57">
+        <v>-81.683865609199998</v>
+      </c>
+      <c r="E57">
+        <v>33.273273141600001</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>174</v>
+      </c>
+      <c r="I57">
+        <v>155</v>
+      </c>
+      <c r="J57">
+        <v>19</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58">
+        <v>436312.94</v>
+      </c>
+      <c r="C58">
+        <v>3681732.75</v>
+      </c>
+      <c r="D58">
+        <v>-81.683696269600006</v>
+      </c>
+      <c r="E58">
+        <v>33.274624150699999</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>168</v>
+      </c>
+      <c r="I58">
+        <v>152</v>
+      </c>
+      <c r="J58">
+        <v>16</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59">
+        <v>436726.43</v>
+      </c>
+      <c r="C59">
+        <v>3681679.46</v>
+      </c>
+      <c r="D59">
+        <v>-81.679252739399999</v>
+      </c>
+      <c r="E59">
+        <v>33.2741678716</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>169</v>
+      </c>
+      <c r="I59">
+        <v>159</v>
+      </c>
+      <c r="J59">
+        <v>10</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60">
+        <v>436679.32</v>
+      </c>
+      <c r="C60">
+        <v>3681448.59</v>
+      </c>
+      <c r="D60">
+        <v>-81.679742460599996</v>
+      </c>
+      <c r="E60">
+        <v>33.272082799700001</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>163</v>
+      </c>
+      <c r="I60">
+        <v>147</v>
+      </c>
+      <c r="J60">
+        <v>16</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61">
+        <v>436674.4</v>
+      </c>
+      <c r="C61">
+        <v>3681369.07</v>
+      </c>
+      <c r="D61">
+        <v>-81.679789736199993</v>
+      </c>
+      <c r="E61">
+        <v>33.271365289400002</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>167</v>
+      </c>
+      <c r="I61">
+        <v>153</v>
+      </c>
+      <c r="J61">
+        <v>14</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62">
+        <v>436734</v>
+      </c>
+      <c r="C62">
+        <v>3681589</v>
+      </c>
+      <c r="D62">
+        <v>-81.679165148300001</v>
+      </c>
+      <c r="E62">
+        <v>33.273352422999999</v>
+      </c>
+      <c r="F62">
+        <v>238</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>166</v>
+      </c>
+      <c r="I62">
+        <v>152</v>
+      </c>
+      <c r="J62">
+        <v>14</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63">
+        <v>436910.98</v>
+      </c>
+      <c r="C63">
+        <v>3681328.41</v>
+      </c>
+      <c r="D63">
+        <v>-81.677246744200005</v>
+      </c>
+      <c r="E63">
+        <v>33.271012438200003</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>177</v>
+      </c>
+      <c r="I63">
+        <v>162</v>
+      </c>
+      <c r="J63">
+        <v>15</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64">
+        <v>436444.92599999998</v>
+      </c>
+      <c r="C64">
+        <v>3681187.8909999998</v>
+      </c>
+      <c r="D64">
+        <v>-81.682240909300006</v>
+      </c>
+      <c r="E64">
+        <v>33.269717657800001</v>
+      </c>
+      <c r="F64">
+        <v>226.1</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>165</v>
+      </c>
+      <c r="I64">
+        <v>148.5</v>
+      </c>
+      <c r="J64">
+        <v>16.5</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65">
+        <v>436723.77</v>
+      </c>
+      <c r="C65">
+        <v>3681318.65</v>
+      </c>
+      <c r="D65">
+        <v>-81.679256132899994</v>
+      </c>
+      <c r="E65">
+        <v>33.270913432199997</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>163</v>
+      </c>
+      <c r="I65">
+        <v>146</v>
+      </c>
+      <c r="J65">
+        <v>17</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" t="s">
+        <v>71</v>
+      </c>
+      <c r="B66">
+        <v>436723.65</v>
+      </c>
+      <c r="C66">
+        <v>3681261.16</v>
+      </c>
+      <c r="D66">
+        <v>-81.6792534115</v>
+      </c>
+      <c r="E66">
+        <v>33.2703949008</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>186</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67">
+        <v>436726.85</v>
+      </c>
+      <c r="C67">
+        <v>3681228.37</v>
+      </c>
+      <c r="D67">
+        <v>-81.679216766600007</v>
+      </c>
+      <c r="E67">
+        <v>33.270099342999998</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>181</v>
+      </c>
+      <c r="I67">
+        <v>166</v>
+      </c>
+      <c r="J67">
+        <v>15</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" t="s">
+        <v>73</v>
+      </c>
+      <c r="B68">
+        <v>436213.45</v>
+      </c>
+      <c r="C68">
+        <v>3681140.37</v>
+      </c>
+      <c r="D68">
+        <v>-81.684722881400006</v>
+      </c>
+      <c r="E68">
+        <v>33.269275372300001</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>185</v>
+      </c>
+      <c r="I68">
+        <v>167</v>
+      </c>
+      <c r="J68">
+        <v>18</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69">
+        <v>436285.62</v>
+      </c>
+      <c r="C69">
+        <v>3681078.66</v>
+      </c>
+      <c r="D69">
+        <v>-81.683943676499993</v>
+      </c>
+      <c r="E69">
+        <v>33.268723055899997</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>186</v>
+      </c>
+      <c r="I69">
+        <v>165</v>
+      </c>
+      <c r="J69">
+        <v>21</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70">
+        <v>436430.22</v>
+      </c>
+      <c r="C70">
+        <v>3681278.32</v>
+      </c>
+      <c r="D70">
+        <v>-81.682405141100006</v>
+      </c>
+      <c r="E70">
+        <v>33.270532403600001</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>163</v>
+      </c>
+      <c r="I70">
+        <v>151</v>
+      </c>
+      <c r="J70">
+        <v>12</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71">
+        <v>436483.95</v>
+      </c>
+      <c r="C71">
+        <v>3681311.7</v>
+      </c>
+      <c r="D71">
+        <v>-81.681830583899995</v>
+      </c>
+      <c r="E71">
+        <v>33.270836638699997</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>165</v>
+      </c>
+      <c r="I71">
+        <v>154</v>
+      </c>
+      <c r="J71">
+        <v>11</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72">
+        <v>436581.4</v>
+      </c>
+      <c r="C72">
+        <v>3681372.57</v>
+      </c>
+      <c r="D72">
+        <v>-81.680788523299995</v>
+      </c>
+      <c r="E72">
+        <v>33.271391387800001</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73">
+        <v>436419.33</v>
+      </c>
+      <c r="C73">
+        <v>3681156.47</v>
+      </c>
+      <c r="D73">
+        <v>-81.682513526799994</v>
+      </c>
+      <c r="E73">
+        <v>33.269432750199996</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>176</v>
+      </c>
+      <c r="I73">
+        <v>156</v>
+      </c>
+      <c r="J73">
+        <v>20</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74">
+        <v>436360.19</v>
+      </c>
+      <c r="C74">
+        <v>3681123.32</v>
+      </c>
+      <c r="D74">
+        <v>-81.683146174300006</v>
+      </c>
+      <c r="E74">
+        <v>33.269130267100003</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>179</v>
+      </c>
+      <c r="I74">
+        <v>161</v>
+      </c>
+      <c r="J74">
+        <v>18</v>
+      </c>
+      <c r="K74">
+        <v>0</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75">
+        <v>436750.62</v>
+      </c>
+      <c r="C75">
+        <v>3681369.15</v>
+      </c>
+      <c r="D75">
+        <v>-81.678971366200003</v>
+      </c>
+      <c r="E75">
+        <v>33.2713704875</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76" t="s">
+        <v>81</v>
+      </c>
+      <c r="B76">
+        <v>436469.09</v>
+      </c>
+      <c r="C76">
+        <v>3681082.64</v>
+      </c>
+      <c r="D76">
+        <v>-81.681974095000001</v>
+      </c>
+      <c r="E76">
+        <v>33.268769784</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+      <c r="K76">
+        <v>0</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77" t="s">
+        <v>82</v>
+      </c>
+      <c r="B77">
+        <v>436425.22</v>
+      </c>
+      <c r="C77">
+        <v>3681053.51</v>
+      </c>
+      <c r="D77">
+        <v>-81.682443072699996</v>
+      </c>
+      <c r="E77">
+        <v>33.268504462499997</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>169</v>
+      </c>
+      <c r="I77">
+        <v>145</v>
+      </c>
+      <c r="J77">
+        <v>24</v>
+      </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
+      <c r="L77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78" t="s">
+        <v>83</v>
+      </c>
+      <c r="B78">
+        <v>436908.23</v>
+      </c>
+      <c r="C78">
+        <v>3681373.7</v>
+      </c>
+      <c r="D78">
+        <v>-81.677279420600001</v>
+      </c>
+      <c r="E78">
+        <v>33.271420765400002</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>171</v>
+      </c>
+      <c r="I78">
+        <v>159</v>
+      </c>
+      <c r="J78">
+        <v>12</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79">
+        <v>436799.94</v>
+      </c>
+      <c r="C79">
+        <v>3681288.05</v>
+      </c>
+      <c r="D79">
+        <v>-81.678436166599994</v>
+      </c>
+      <c r="E79">
+        <v>33.270641908999998</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>177</v>
+      </c>
+      <c r="I79">
+        <v>162</v>
+      </c>
+      <c r="J79">
+        <v>15</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80">
+        <v>436549.88</v>
+      </c>
+      <c r="C80">
+        <v>3681172.45</v>
+      </c>
+      <c r="D80">
+        <v>-81.681112958100002</v>
+      </c>
+      <c r="E80">
+        <v>33.269584574100001</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>172</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81" t="s">
+        <v>86</v>
+      </c>
+      <c r="B81">
+        <v>436529.81</v>
+      </c>
+      <c r="C81">
+        <v>3681140.09</v>
+      </c>
+      <c r="D81">
+        <v>-81.681326181800003</v>
+      </c>
+      <c r="E81">
+        <v>33.269291525100002</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>182</v>
+      </c>
+      <c r="I81">
+        <v>161</v>
+      </c>
+      <c r="J81">
+        <v>21</v>
+      </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
+      <c r="L81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="A82" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82">
+        <v>436689.4</v>
+      </c>
+      <c r="C82">
+        <v>3681194.35</v>
+      </c>
+      <c r="D82">
+        <v>-81.679616488099995</v>
+      </c>
+      <c r="E82">
+        <v>33.269790304099999</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>174</v>
+      </c>
+      <c r="I82">
+        <v>152</v>
+      </c>
+      <c r="J82">
+        <v>22</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+      <c r="L82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="A83" t="s">
+        <v>88</v>
+      </c>
+      <c r="B83">
+        <v>436787.87</v>
+      </c>
+      <c r="C83">
+        <v>3681319.92</v>
+      </c>
+      <c r="D83">
+        <v>-81.678567982000004</v>
+      </c>
+      <c r="E83">
+        <v>33.270928648899996</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>174</v>
+      </c>
+      <c r="I83">
+        <v>156</v>
+      </c>
+      <c r="J83">
+        <v>18</v>
+      </c>
+      <c r="K83">
+        <v>0</v>
+      </c>
+      <c r="L83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="A84" t="s">
+        <v>89</v>
+      </c>
+      <c r="B84">
+        <v>436875.86</v>
+      </c>
+      <c r="C84">
+        <v>3681365.57</v>
+      </c>
+      <c r="D84">
+        <v>-81.677626412600006</v>
+      </c>
+      <c r="E84">
+        <v>33.271345541999999</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>162</v>
+      </c>
+      <c r="I84">
+        <v>145</v>
+      </c>
+      <c r="J84">
+        <v>17</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="A85" t="s">
+        <v>90</v>
+      </c>
+      <c r="B85">
+        <v>436793.08</v>
+      </c>
+      <c r="C85">
+        <v>3681354.97</v>
+      </c>
+      <c r="D85">
+        <v>-81.678514484399997</v>
+      </c>
+      <c r="E85">
+        <v>33.271245084</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>170</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="A86" t="s">
+        <v>91</v>
+      </c>
+      <c r="B86">
+        <v>436789.45899999997</v>
+      </c>
+      <c r="C86">
+        <v>3681398.0890000002</v>
+      </c>
+      <c r="D86">
+        <v>-81.678556367499993</v>
+      </c>
+      <c r="E86">
+        <v>33.271633778499996</v>
+      </c>
+      <c r="F86">
+        <v>230.62</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>164.75</v>
+      </c>
+      <c r="I86">
+        <v>153.75</v>
+      </c>
+      <c r="J86">
+        <v>11</v>
+      </c>
+      <c r="K86">
+        <v>0</v>
+      </c>
+      <c r="L86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="A87" t="s">
+        <v>92</v>
+      </c>
+      <c r="B87">
+        <v>436975.13</v>
+      </c>
+      <c r="C87">
+        <v>3681442.81</v>
+      </c>
+      <c r="D87">
+        <v>-81.676565914700006</v>
+      </c>
+      <c r="E87">
+        <v>33.272048010399999</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>171</v>
+      </c>
+      <c r="I87">
+        <v>156</v>
+      </c>
+      <c r="J87">
+        <v>15</v>
+      </c>
+      <c r="K87">
+        <v>0</v>
+      </c>
+      <c r="L87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
+      <c r="A88" t="s">
+        <v>93</v>
+      </c>
+      <c r="B88">
+        <v>436946.1</v>
+      </c>
+      <c r="C88">
+        <v>3681421.44</v>
+      </c>
+      <c r="D88">
+        <v>-81.676876127499995</v>
+      </c>
+      <c r="E88">
+        <v>33.271853567699999</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>172</v>
+      </c>
+      <c r="I88">
+        <v>156</v>
+      </c>
+      <c r="J88">
+        <v>16</v>
+      </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
+      <c r="L88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
+      <c r="A89" t="s">
+        <v>94</v>
+      </c>
+      <c r="B89">
+        <v>436910.46</v>
+      </c>
+      <c r="C89">
+        <v>3681351.73</v>
+      </c>
+      <c r="D89">
+        <v>-81.677253949199994</v>
+      </c>
+      <c r="E89">
+        <v>33.271222739999999</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>174</v>
+      </c>
+      <c r="I89">
+        <v>162</v>
+      </c>
+      <c r="J89">
+        <v>12</v>
+      </c>
+      <c r="K89">
+        <v>0</v>
+      </c>
+      <c r="L89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
+      <c r="A90" t="s">
+        <v>95</v>
+      </c>
+      <c r="B90">
+        <v>436892.52</v>
+      </c>
+      <c r="C90">
+        <v>3681306.3</v>
+      </c>
+      <c r="D90">
+        <v>-81.677443410799995</v>
+      </c>
+      <c r="E90">
+        <v>33.270811938599998</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>172</v>
+      </c>
+      <c r="I90">
+        <v>157</v>
+      </c>
+      <c r="J90">
+        <v>15</v>
+      </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
+      <c r="L90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
+      <c r="A91" t="s">
+        <v>96</v>
+      </c>
+      <c r="B91">
+        <v>436901.13</v>
+      </c>
+      <c r="C91">
+        <v>3681258.14</v>
+      </c>
+      <c r="D91">
+        <v>-81.677347616000006</v>
+      </c>
+      <c r="E91">
+        <v>33.270378069000003</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>178</v>
+      </c>
+      <c r="I91">
+        <v>162</v>
+      </c>
+      <c r="J91">
+        <v>16</v>
+      </c>
+      <c r="K91">
+        <v>0</v>
+      </c>
+      <c r="L91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
+      <c r="A92" t="s">
+        <v>97</v>
+      </c>
+      <c r="B92">
+        <v>436843.31</v>
+      </c>
+      <c r="C92">
+        <v>3681353.37</v>
+      </c>
+      <c r="D92">
+        <v>-81.677975053200001</v>
+      </c>
+      <c r="E92">
+        <v>33.271233598199998</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>164</v>
+      </c>
+      <c r="I92">
+        <v>150</v>
+      </c>
+      <c r="J92">
+        <v>14</v>
+      </c>
+      <c r="K92">
+        <v>0</v>
+      </c>
+      <c r="L92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
+      <c r="A93" t="s">
+        <v>98</v>
+      </c>
+      <c r="B93">
+        <v>436765.58</v>
+      </c>
+      <c r="C93">
+        <v>3681291.63</v>
+      </c>
+      <c r="D93">
+        <v>-81.678805337100002</v>
+      </c>
+      <c r="E93">
+        <v>33.270672182699997</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93">
+        <v>180</v>
+      </c>
+      <c r="I93">
+        <v>167</v>
+      </c>
+      <c r="J93">
+        <v>13</v>
+      </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
+      <c r="L93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="A94" t="s">
+        <v>99</v>
+      </c>
+      <c r="B94">
+        <v>436822.71</v>
+      </c>
+      <c r="C94">
+        <v>3681272.68</v>
+      </c>
+      <c r="D94">
+        <v>-81.6781906163</v>
+      </c>
+      <c r="E94">
+        <v>33.2705046162</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>189</v>
+      </c>
+      <c r="I94">
+        <v>174</v>
+      </c>
+      <c r="J94">
+        <v>15</v>
+      </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
+      <c r="L94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
+      <c r="A95" t="s">
+        <v>100</v>
+      </c>
+      <c r="B95">
+        <v>436415.78</v>
+      </c>
+      <c r="C95">
+        <v>3681120.3</v>
+      </c>
+      <c r="D95">
+        <v>-81.682549107499995</v>
+      </c>
+      <c r="E95">
+        <v>33.269106309800001</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>177</v>
+      </c>
+      <c r="I95">
+        <v>155</v>
+      </c>
+      <c r="J95">
+        <v>22</v>
+      </c>
+      <c r="K95">
+        <v>0</v>
+      </c>
+      <c r="L95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
+      <c r="A96" t="s">
+        <v>101</v>
+      </c>
+      <c r="B96">
+        <v>436736.56</v>
+      </c>
+      <c r="C96">
+        <v>3681194.99</v>
+      </c>
+      <c r="D96">
+        <v>-81.679110183999995</v>
+      </c>
+      <c r="E96">
+        <v>33.269798846</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>180</v>
+      </c>
+      <c r="I96">
+        <v>160</v>
+      </c>
+      <c r="J96">
+        <v>20</v>
+      </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
+      <c r="L96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
+      <c r="A97" t="s">
+        <v>102</v>
+      </c>
+      <c r="B97">
+        <v>436836.51199999999</v>
+      </c>
+      <c r="C97">
+        <v>3681433.1860000002</v>
+      </c>
+      <c r="D97">
+        <v>-81.678053600699997</v>
+      </c>
+      <c r="E97">
+        <v>33.271953091100002</v>
+      </c>
+      <c r="F97">
+        <v>229.68</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>171</v>
+      </c>
+      <c r="I97">
+        <v>154</v>
+      </c>
+      <c r="J97">
+        <v>17</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="L97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
+      <c r="A98" t="s">
+        <v>103</v>
+      </c>
+      <c r="B98">
+        <v>436726.35</v>
+      </c>
+      <c r="C98">
+        <v>3681243.15</v>
+      </c>
+      <c r="D98">
+        <v>-81.679223165799996</v>
+      </c>
+      <c r="E98">
+        <v>33.270232620199998</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>188</v>
+      </c>
+      <c r="I98">
+        <v>0</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
+      <c r="A99" t="s">
+        <v>104</v>
+      </c>
+      <c r="B99">
+        <v>436698.93</v>
+      </c>
+      <c r="C99">
+        <v>3681233.25</v>
+      </c>
+      <c r="D99">
+        <v>-81.6795168803</v>
+      </c>
+      <c r="E99">
+        <v>33.270141717999998</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>184</v>
+      </c>
+      <c r="I99">
+        <v>0</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+      <c r="K99">
+        <v>0</v>
+      </c>
+      <c r="L99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
+      <c r="A100" t="s">
+        <v>105</v>
+      </c>
+      <c r="B100">
+        <v>436704.7</v>
+      </c>
+      <c r="C100">
+        <v>3681258.07</v>
+      </c>
+      <c r="D100">
+        <v>-81.679456660200003</v>
+      </c>
+      <c r="E100">
+        <v>33.270365918000003</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>177</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+      <c r="K100">
+        <v>0</v>
+      </c>
+      <c r="L100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
+      <c r="A101" t="s">
+        <v>106</v>
+      </c>
+      <c r="B101">
+        <v>436669.82</v>
+      </c>
+      <c r="C101">
+        <v>3681227.7</v>
+      </c>
+      <c r="D101">
+        <v>-81.6798290431</v>
+      </c>
+      <c r="E101">
+        <v>33.270089950100001</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>169</v>
+      </c>
+      <c r="I101">
+        <v>156</v>
+      </c>
+      <c r="J101">
+        <v>13</v>
+      </c>
+      <c r="K101">
+        <v>0</v>
+      </c>
+      <c r="L101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
+      <c r="A102" t="s">
+        <v>107</v>
+      </c>
+      <c r="B102">
+        <v>436648.53</v>
+      </c>
+      <c r="C102">
+        <v>3681205.83</v>
+      </c>
+      <c r="D102">
+        <v>-81.680056103799998</v>
+      </c>
+      <c r="E102">
+        <v>33.269891444800002</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <v>174</v>
+      </c>
+      <c r="I102">
+        <v>158</v>
+      </c>
+      <c r="J102">
+        <v>16</v>
+      </c>
+      <c r="K102">
+        <v>0</v>
+      </c>
+      <c r="L102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
+      <c r="A103" t="s">
+        <v>108</v>
+      </c>
+      <c r="B103">
+        <v>436596.17</v>
+      </c>
+      <c r="C103">
+        <v>3681214.59</v>
+      </c>
+      <c r="D103">
+        <v>-81.680618896699997</v>
+      </c>
+      <c r="E103">
+        <v>33.269967375199997</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <v>186</v>
+      </c>
+      <c r="I103">
+        <v>0</v>
+      </c>
+      <c r="J103">
+        <v>0</v>
+      </c>
+      <c r="K103">
+        <v>0</v>
+      </c>
+      <c r="L103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
+      <c r="A104" t="s">
+        <v>109</v>
+      </c>
+      <c r="B104">
+        <v>436583.15</v>
+      </c>
+      <c r="C104">
+        <v>3681067.41</v>
+      </c>
+      <c r="D104">
+        <v>-81.680748402899994</v>
+      </c>
+      <c r="E104">
+        <v>33.268639136399997</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+      <c r="H104">
+        <v>185</v>
+      </c>
+      <c r="I104">
+        <v>0</v>
+      </c>
+      <c r="J104">
+        <v>0</v>
+      </c>
+      <c r="K104">
+        <v>0</v>
+      </c>
+      <c r="L104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
+      <c r="A105" t="s">
+        <v>110</v>
+      </c>
+      <c r="B105">
+        <v>436719.75</v>
+      </c>
+      <c r="C105">
+        <v>3682122.61</v>
+      </c>
+      <c r="D105">
+        <v>-81.679355383900003</v>
+      </c>
+      <c r="E105">
+        <v>33.278164415799999</v>
+      </c>
+      <c r="F105">
+        <v>293.3</v>
+      </c>
+      <c r="G105">
+        <v>276</v>
+      </c>
+      <c r="H105">
+        <v>190</v>
+      </c>
+      <c r="I105">
+        <v>185.3</v>
+      </c>
+      <c r="J105">
+        <v>4.7</v>
+      </c>
+      <c r="K105">
+        <v>153</v>
+      </c>
+      <c r="L105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
+      <c r="A106" t="s">
+        <v>111</v>
+      </c>
+      <c r="B106">
+        <v>436719.95</v>
+      </c>
+      <c r="C106">
+        <v>3682034.37</v>
+      </c>
+      <c r="D106">
+        <v>-81.679347079300001</v>
+      </c>
+      <c r="E106">
+        <v>33.277368557999999</v>
+      </c>
+      <c r="F106">
+        <v>290.5</v>
+      </c>
+      <c r="G106">
+        <v>267</v>
+      </c>
+      <c r="H106">
+        <v>189</v>
+      </c>
+      <c r="I106">
+        <v>179.5</v>
+      </c>
+      <c r="J106">
+        <v>9.5</v>
+      </c>
+      <c r="K106">
+        <v>153</v>
+      </c>
+      <c r="L106">
+        <v>118.923</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12">
+      <c r="A107" t="s">
+        <v>112</v>
+      </c>
+      <c r="B107">
+        <v>436736.1</v>
+      </c>
+      <c r="C107">
+        <v>3681895</v>
+      </c>
+      <c r="D107">
+        <v>-81.679163942900004</v>
+      </c>
+      <c r="E107">
+        <v>33.276112476199998</v>
+      </c>
+      <c r="F107">
+        <v>283.8</v>
+      </c>
+      <c r="G107">
+        <v>261</v>
+      </c>
+      <c r="H107">
+        <v>185</v>
+      </c>
+      <c r="I107">
+        <v>182.8</v>
+      </c>
+      <c r="J107">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K107">
+        <v>150</v>
+      </c>
+      <c r="L107">
+        <v>115.8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12">
+      <c r="A108" t="s">
+        <v>113</v>
+      </c>
+      <c r="B108">
+        <v>436440</v>
+      </c>
+      <c r="C108">
+        <v>3681189</v>
+      </c>
+      <c r="D108">
+        <v>-81.682293876499998</v>
+      </c>
+      <c r="E108">
+        <v>33.269727369800002</v>
+      </c>
+      <c r="F108">
+        <v>227</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+      <c r="H108">
+        <v>164</v>
+      </c>
+      <c r="I108">
+        <v>144</v>
+      </c>
+      <c r="J108">
+        <v>20</v>
+      </c>
+      <c r="K108">
+        <v>131</v>
+      </c>
+      <c r="L108">
+        <v>102.884</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
+      <c r="A109" t="s">
+        <v>114</v>
+      </c>
+      <c r="B109">
+        <v>437007.48800000001</v>
+      </c>
+      <c r="C109">
+        <v>3681579.1179999998</v>
+      </c>
+      <c r="D109">
+        <v>-81.676227948800005</v>
+      </c>
+      <c r="E109">
+        <v>33.2732793176</v>
+      </c>
+      <c r="F109">
+        <v>221.3</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+      <c r="H109">
+        <v>178</v>
+      </c>
+      <c r="I109">
+        <v>171</v>
+      </c>
+      <c r="J109">
+        <v>7</v>
+      </c>
+      <c r="K109">
+        <v>0</v>
+      </c>
+      <c r="L109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12">
+      <c r="A110" t="s">
+        <v>115</v>
+      </c>
+      <c r="B110">
+        <v>437046.2</v>
+      </c>
+      <c r="C110">
+        <v>3682032</v>
+      </c>
+      <c r="D110">
+        <v>-81.675843721700005</v>
+      </c>
+      <c r="E110">
+        <v>33.277366298399997</v>
+      </c>
+      <c r="F110">
+        <v>250</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+      <c r="H110">
+        <v>178</v>
+      </c>
+      <c r="I110">
+        <v>173</v>
+      </c>
+      <c r="J110">
+        <v>5</v>
+      </c>
+      <c r="K110">
+        <v>147</v>
+      </c>
+      <c r="L110">
+        <v>112.85599999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12">
+      <c r="A111" t="s">
+        <v>116</v>
+      </c>
+      <c r="B111">
+        <v>436975.8</v>
+      </c>
+      <c r="C111">
+        <v>3680933</v>
+      </c>
+      <c r="D111">
+        <v>-81.676523306000007</v>
+      </c>
+      <c r="E111">
+        <v>33.267449872599997</v>
+      </c>
+      <c r="F111">
+        <v>205.8</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <v>181</v>
+      </c>
+      <c r="I111">
+        <v>173.8</v>
+      </c>
+      <c r="J111">
+        <v>7.2</v>
+      </c>
+      <c r="K111">
+        <v>140</v>
+      </c>
+      <c r="L111">
+        <v>101.82899999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12">
+      <c r="A112" t="s">
+        <v>117</v>
+      </c>
+      <c r="B112">
+        <v>437162.07299999997</v>
+      </c>
+      <c r="C112">
+        <v>3681148.1660000002</v>
+      </c>
+      <c r="D112">
+        <v>-81.674538278499995</v>
+      </c>
+      <c r="E112">
+        <v>33.269401417300003</v>
+      </c>
+      <c r="F112">
+        <v>200.5</v>
+      </c>
+      <c r="G112">
+        <v>0</v>
+      </c>
+      <c r="H112">
+        <v>176</v>
+      </c>
+      <c r="I112">
+        <v>171</v>
+      </c>
+      <c r="J112">
+        <v>5</v>
+      </c>
+      <c r="K112">
+        <v>0</v>
+      </c>
+      <c r="L112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
+      <c r="A113" t="s">
+        <v>118</v>
+      </c>
+      <c r="B113">
+        <v>436295.4</v>
+      </c>
+      <c r="C113">
+        <v>3681577</v>
+      </c>
+      <c r="D113">
+        <v>-81.683873665299998</v>
+      </c>
+      <c r="E113">
+        <v>33.273218347300002</v>
+      </c>
+      <c r="F113">
+        <v>278</v>
+      </c>
+      <c r="G113">
+        <v>235</v>
+      </c>
+      <c r="H113">
+        <v>181</v>
+      </c>
+      <c r="I113">
+        <v>165</v>
+      </c>
+      <c r="J113">
+        <v>16</v>
+      </c>
+      <c r="K113">
+        <v>139</v>
+      </c>
+      <c r="L113">
+        <v>111.518</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
+      <c r="A114" t="s">
+        <v>119</v>
+      </c>
+      <c r="B114">
+        <v>436176.21</v>
+      </c>
+      <c r="C114">
+        <v>3681346.43</v>
+      </c>
+      <c r="D114">
+        <v>-81.685137214099996</v>
+      </c>
+      <c r="E114">
+        <v>33.2711316985</v>
+      </c>
+      <c r="F114">
+        <v>254.4</v>
+      </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+      <c r="H114">
+        <v>173</v>
+      </c>
+      <c r="I114">
+        <v>162</v>
+      </c>
+      <c r="J114">
+        <v>11</v>
+      </c>
+      <c r="K114">
+        <v>0</v>
+      </c>
+      <c r="L114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
+      <c r="A115" t="s">
+        <v>120</v>
+      </c>
+      <c r="B115">
+        <v>436350.93</v>
+      </c>
+      <c r="C115">
+        <v>3680993.49</v>
+      </c>
+      <c r="D115">
+        <v>-81.683236488899993</v>
+      </c>
+      <c r="E115">
+        <v>33.267958734700002</v>
+      </c>
+      <c r="F115">
+        <v>216</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>181</v>
+      </c>
+      <c r="I115">
+        <v>173</v>
+      </c>
+      <c r="J115">
+        <v>8</v>
+      </c>
+      <c r="K115">
+        <v>0</v>
+      </c>
+      <c r="L115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
+      <c r="A116" t="s">
+        <v>121</v>
+      </c>
+      <c r="B116">
+        <v>436681.8</v>
+      </c>
+      <c r="C116">
+        <v>3681563</v>
+      </c>
+      <c r="D116">
+        <v>-81.679723818400007</v>
+      </c>
+      <c r="E116">
+        <v>33.273114852699997</v>
+      </c>
+      <c r="F116">
+        <v>270.5</v>
+      </c>
+      <c r="G116">
+        <v>228</v>
+      </c>
+      <c r="H116">
+        <v>163</v>
+      </c>
+      <c r="I116">
+        <v>160.5</v>
+      </c>
+      <c r="J116">
+        <v>2.5</v>
+      </c>
+      <c r="K116">
+        <v>132.5</v>
+      </c>
+      <c r="L116">
+        <v>100.5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
+      <c r="A117" t="s">
+        <v>122</v>
+      </c>
+      <c r="B117">
+        <v>436871.9</v>
+      </c>
+      <c r="C117">
+        <v>3681290</v>
+      </c>
+      <c r="D117">
+        <v>-81.677663672600005</v>
+      </c>
+      <c r="E117">
+        <v>33.270663714800001</v>
+      </c>
+      <c r="F117">
+        <v>216.1</v>
+      </c>
+      <c r="G117">
+        <v>0</v>
+      </c>
+      <c r="H117">
+        <v>173</v>
+      </c>
+      <c r="I117">
+        <v>164.1</v>
+      </c>
+      <c r="J117">
+        <v>8.9</v>
+      </c>
+      <c r="K117">
+        <v>134</v>
+      </c>
+      <c r="L117">
+        <v>103.1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
+      <c r="A118" t="s">
+        <v>123</v>
+      </c>
+      <c r="B118">
+        <v>436516.4</v>
+      </c>
+      <c r="C118">
+        <v>3681762</v>
+      </c>
+      <c r="D118">
+        <v>-81.6815136835</v>
+      </c>
+      <c r="E118">
+        <v>33.274899975399997</v>
+      </c>
+      <c r="F118">
+        <v>285.60000000000002</v>
+      </c>
+      <c r="G118">
+        <v>255</v>
+      </c>
+      <c r="H118">
+        <v>176</v>
+      </c>
+      <c r="I118">
+        <v>172.6</v>
+      </c>
+      <c r="J118">
+        <v>3.4</v>
+      </c>
+      <c r="K118">
+        <v>135</v>
+      </c>
+      <c r="L118">
+        <v>111.14100000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
+      <c r="A119" t="s">
+        <v>124</v>
+      </c>
+      <c r="B119">
+        <v>436562.3</v>
+      </c>
+      <c r="C119">
+        <v>3681523</v>
+      </c>
+      <c r="D119">
+        <v>-81.681004119999997</v>
+      </c>
+      <c r="E119">
+        <v>33.272747048500001</v>
+      </c>
+      <c r="F119">
+        <v>277.7</v>
+      </c>
+      <c r="G119">
+        <v>234</v>
+      </c>
+      <c r="H119">
+        <v>167</v>
+      </c>
+      <c r="I119">
+        <v>153.69999999999999</v>
+      </c>
+      <c r="J119">
+        <v>13.3</v>
+      </c>
+      <c r="K119">
+        <v>135.69999999999999</v>
+      </c>
+      <c r="L119">
+        <v>103.7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
+      <c r="A120" t="s">
+        <v>125</v>
+      </c>
+      <c r="B120">
+        <v>436556.5</v>
+      </c>
+      <c r="C120">
+        <v>3681628</v>
+      </c>
+      <c r="D120">
+        <v>-81.681073739400006</v>
+      </c>
+      <c r="E120">
+        <v>33.273693741400002</v>
+      </c>
+      <c r="F120">
+        <v>283.8</v>
+      </c>
+      <c r="G120">
+        <v>244.8</v>
+      </c>
+      <c r="H120">
+        <v>163</v>
+      </c>
+      <c r="I120">
+        <v>151.80000000000001</v>
+      </c>
+      <c r="J120">
+        <v>11.2</v>
+      </c>
+      <c r="K120">
+        <v>137.80000000000001</v>
+      </c>
+      <c r="L120">
+        <v>107.8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
+      <c r="A121" t="s">
+        <v>126</v>
+      </c>
+      <c r="B121">
+        <v>436555.2</v>
+      </c>
+      <c r="C121">
+        <v>3681710</v>
+      </c>
+      <c r="D121">
+        <v>-81.681093433399994</v>
+      </c>
+      <c r="E121">
+        <v>33.274433253600002</v>
+      </c>
+      <c r="F121">
+        <v>280.7</v>
+      </c>
+      <c r="G121">
+        <v>242</v>
+      </c>
+      <c r="H121">
+        <v>172</v>
+      </c>
+      <c r="I121">
+        <v>168.7</v>
+      </c>
+      <c r="J121">
+        <v>3.3</v>
+      </c>
+      <c r="K121">
+        <v>135</v>
+      </c>
+      <c r="L121">
+        <v>107.7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
+      <c r="A122" t="s">
+        <v>127</v>
+      </c>
+      <c r="B122">
+        <v>436552.1</v>
+      </c>
+      <c r="C122">
+        <v>3681815</v>
+      </c>
+      <c r="D122">
+        <v>-81.681134064099993</v>
+      </c>
+      <c r="E122">
+        <v>33.2753801052</v>
+      </c>
+      <c r="F122">
+        <v>285.3</v>
+      </c>
+      <c r="G122">
+        <v>247</v>
+      </c>
+      <c r="H122">
+        <v>178</v>
+      </c>
+      <c r="I122">
+        <v>173.3</v>
+      </c>
+      <c r="J122">
+        <v>4.7</v>
+      </c>
+      <c r="K122">
+        <v>137</v>
+      </c>
+      <c r="L122">
+        <v>113.32899999999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
+      <c r="A123" t="s">
+        <v>128</v>
+      </c>
+      <c r="B123">
+        <v>436719.81530000002</v>
+      </c>
+      <c r="C123">
+        <v>3681887.2</v>
+      </c>
+      <c r="D123">
+        <v>-81.679338257200001</v>
+      </c>
+      <c r="E123">
+        <v>33.276041168600003</v>
+      </c>
+      <c r="F123">
+        <v>287.39999399999999</v>
+      </c>
+      <c r="G123">
+        <v>0</v>
+      </c>
+      <c r="H123">
+        <v>180</v>
+      </c>
+      <c r="I123">
+        <v>164</v>
+      </c>
+      <c r="J123">
+        <v>16</v>
+      </c>
+      <c r="K123">
+        <v>0</v>
+      </c>
+      <c r="L123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12">
+      <c r="A124" t="s">
+        <v>129</v>
+      </c>
+      <c r="B124">
+        <v>436613.38809999998</v>
+      </c>
+      <c r="C124">
+        <v>3681917.22</v>
+      </c>
+      <c r="D124">
+        <v>-81.680483126699997</v>
+      </c>
+      <c r="E124">
+        <v>33.276305673300001</v>
+      </c>
+      <c r="F124">
+        <v>294.89999399999999</v>
+      </c>
+      <c r="G124">
+        <v>0</v>
+      </c>
+      <c r="H124">
+        <v>188</v>
+      </c>
+      <c r="I124">
+        <v>176</v>
+      </c>
+      <c r="J124">
+        <v>12</v>
+      </c>
+      <c r="K124">
+        <v>0</v>
+      </c>
+      <c r="L124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12">
+      <c r="A125" t="s">
+        <v>130</v>
+      </c>
+      <c r="B125">
+        <v>436569.38140000001</v>
+      </c>
+      <c r="C125">
+        <v>3681890.53</v>
+      </c>
+      <c r="D125">
+        <v>-81.680953787199996</v>
+      </c>
+      <c r="E125">
+        <v>33.276062355999997</v>
+      </c>
+      <c r="F125">
+        <v>290.70001200000002</v>
+      </c>
+      <c r="G125">
+        <v>0</v>
+      </c>
+      <c r="H125">
+        <v>187</v>
+      </c>
+      <c r="I125">
+        <v>176</v>
+      </c>
+      <c r="J125">
+        <v>11</v>
+      </c>
+      <c r="K125">
+        <v>0</v>
+      </c>
+      <c r="L125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12">
+      <c r="A126" t="s">
+        <v>131</v>
+      </c>
+      <c r="B126">
+        <v>436495.28989999997</v>
+      </c>
+      <c r="C126">
+        <v>3681841.65</v>
+      </c>
+      <c r="D126">
+        <v>-81.681745928699996</v>
+      </c>
+      <c r="E126">
+        <v>33.275617124100002</v>
+      </c>
+      <c r="F126">
+        <v>283.89999399999999</v>
+      </c>
+      <c r="G126">
+        <v>0</v>
+      </c>
+      <c r="H126">
+        <v>179</v>
+      </c>
+      <c r="I126">
+        <v>162</v>
+      </c>
+      <c r="J126">
+        <v>17</v>
+      </c>
+      <c r="K126">
+        <v>0</v>
+      </c>
+      <c r="L126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12">
+      <c r="A127" t="s">
+        <v>132</v>
+      </c>
+      <c r="B127">
+        <v>436726.79389999999</v>
+      </c>
+      <c r="C127">
+        <v>3681978.63</v>
+      </c>
+      <c r="D127">
+        <v>-81.679269702400006</v>
+      </c>
+      <c r="E127">
+        <v>33.276866220099997</v>
+      </c>
+      <c r="F127">
+        <v>287.5</v>
+      </c>
+      <c r="G127">
+        <v>0</v>
+      </c>
+      <c r="H127">
+        <v>194</v>
+      </c>
+      <c r="I127">
+        <v>177</v>
+      </c>
+      <c r="J127">
+        <v>17</v>
+      </c>
+      <c r="K127">
+        <v>0</v>
+      </c>
+      <c r="L127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12">
+      <c r="A128" t="s">
+        <v>133</v>
+      </c>
+      <c r="B128">
+        <v>436792.71100000001</v>
+      </c>
+      <c r="C128">
+        <v>3681393.6379999998</v>
+      </c>
+      <c r="D128">
+        <v>-81.678521140499996</v>
+      </c>
+      <c r="E128">
+        <v>33.271593824</v>
+      </c>
+      <c r="F128">
+        <v>230.8</v>
+      </c>
+      <c r="G128">
+        <v>0</v>
+      </c>
+      <c r="H128">
+        <v>161</v>
+      </c>
+      <c r="I128">
+        <v>157</v>
+      </c>
+      <c r="J128">
+        <v>4</v>
+      </c>
+      <c r="K128">
+        <v>0</v>
+      </c>
+      <c r="L128">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>